<commit_message>
added files for SRAM optimizations
</commit_message>
<xml_diff>
--- a/SPI-Connection-Manuca-FPGA/PinMapping.xlsx
+++ b/SPI-Connection-Manuca-FPGA/PinMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9530a7e920cdbb2/_My Melina/Studium/9.Semester/Forschungspraxis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e9530a7e920cdbb2/_My Melina/Studium/9.Semester/Forschungspraxis/GitHub/Research-Internship-NUS/SPI-Connection-Manuca-FPGA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{091832B5-C9F5-EC48-8B7E-AD0BD7E16B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F64F039-3528-914B-98A7-E5AA3A05C3B5}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{091832B5-C9F5-EC48-8B7E-AD0BD7E16B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24A8E508-A6A7-5F4B-876F-976D5F5AFCEE}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{5F47B0D7-F7BF-9247-9EB4-232A0D802468}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{5F47B0D7-F7BF-9247-9EB4-232A0D802468}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Pin Name</t>
   </si>
   <si>
-    <t>Manuca Board</t>
-  </si>
-  <si>
     <t>FMC XM105 Debug Card</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>CN301.1 (PC10)</t>
   </si>
   <si>
-    <t>CN201.32 (PA4)</t>
-  </si>
-  <si>
     <t>CN405.3</t>
   </si>
   <si>
@@ -225,7 +219,13 @@
     <t>CN405.4</t>
   </si>
   <si>
-    <t xml:space="preserve">Manuca </t>
+    <t>CN301.32 (PA4)</t>
+  </si>
+  <si>
+    <t>Manuca 3.3V</t>
+  </si>
+  <si>
+    <t>Manuca 5V</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,223 +632,223 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
         <v>57</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="G12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>